<commit_message>
Dropped in WRI's input data for first draft of 2.1. made several fixes to model run errors
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,40 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\India EPS\InputData UPDATE FOR INDIA\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\Input Data for India 2.0\add-outputs\VoaSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52975A89-5BC0-4058-80CA-CA22069465FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24915" windowHeight="11580"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="India Data" sheetId="4" r:id="rId2"/>
     <sheet name="VoaSL" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
   <si>
     <t>VoaSL Value of a Statistical Life</t>
   </si>
   <si>
-    <t>Source:</t>
-  </si>
-  <si>
-    <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
-  </si>
-  <si>
-    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -56,9 +56,6 @@
     <t>variable for the result to be accurate.</t>
   </si>
   <si>
-    <t>Currency Year Adjustment</t>
-  </si>
-  <si>
     <t>Page 9, Table 3</t>
   </si>
   <si>
@@ -71,21 +68,12 @@
     <t>Value of Statistical Life: A Meta-Analysis with Mixed Effects Regression Model</t>
   </si>
   <si>
-    <t>The cited study is a meta-analysis of other studies.  There are three values</t>
-  </si>
-  <si>
-    <t>from studies done in India:</t>
-  </si>
-  <si>
     <t>Study</t>
   </si>
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Currency</t>
   </si>
   <si>
@@ -119,12 +107,6 @@
     <t>Year (U.S. dollars)</t>
   </si>
   <si>
-    <t>Exhange Rate</t>
-  </si>
-  <si>
-    <t>2004 Ruppees per 2004 Dollar</t>
-  </si>
-  <si>
     <t>see scaling-factors.xlsx for source info</t>
   </si>
   <si>
@@ -137,31 +119,133 @@
     <t>Selected VoaSL</t>
   </si>
   <si>
-    <t>The India team regards the third data point (nearly $6 million 2012 USD) as being unrealistically</t>
-  </si>
-  <si>
-    <t>high, so we discard it as an ourlier.  We take an average of the other two data points to obtain</t>
-  </si>
-  <si>
-    <t>our selected VoaSL value.</t>
-  </si>
-  <si>
     <t>http://www.sviva.gov.il/english/env_topics/airquality/pollutionfromtransportation/documents/the-cost-of-air-pollution-oecd-report-2014.pdf</t>
   </si>
   <si>
-    <t>Also, an OECD source that uses VoaSL values well under $1 million for India is:</t>
+    <t>Agamomi Majumder &amp; S Madeshwaran</t>
+  </si>
+  <si>
+    <t>Shanmugam</t>
+  </si>
+  <si>
+    <t>INR (assumed to be 1997)</t>
+  </si>
+  <si>
+    <t>INR (assumed to be 2001)</t>
+  </si>
+  <si>
+    <t>INR (assumed to be 2010)</t>
+  </si>
+  <si>
+    <t>Page 3</t>
+  </si>
+  <si>
+    <t>INR (assumed to be 2016)</t>
+  </si>
+  <si>
+    <t>Exhange Rate (INR per USD)</t>
+  </si>
+  <si>
+    <t>http://www.isec.ac.in/WP%20407%20-%20Agamoni%20Majumder%20and%20Madheswaran%20-%20Final.pdf</t>
+  </si>
+  <si>
+    <t>Abstract, Page 1</t>
+  </si>
+  <si>
+    <t>Value of Statistical Life: A Hedonic Wage Approach</t>
+  </si>
+  <si>
+    <t>The previous version of the model used an average of available estimates from Source 1 i.e. the meta-analysis study</t>
+  </si>
+  <si>
+    <t>The same authors have released an updated working paper in 2018, which lists more historic sources and</t>
+  </si>
+  <si>
+    <t>the evolution of the underlying assumptions used across these estimates</t>
+  </si>
+  <si>
+    <t>Indian labour market since the 90s, and the change in patterns in job risk, fatal industrial incidents,</t>
+  </si>
+  <si>
+    <t>reflective of the changes mentioned above</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>| &lt;-- Source 1 (2016)</t>
+  </si>
+  <si>
+    <t>| &lt;--- Source 2 (2018)</t>
+  </si>
+  <si>
+    <t>Range of estimates from studies reviewed in Sources 1 and 2:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and job risk preferences of workers - the 2018 estimate is thus higher. We use this estimate as it is </t>
+  </si>
+  <si>
+    <t>Table 2.17. Page 61</t>
+  </si>
+  <si>
+    <t>Value (Millions)</t>
+  </si>
+  <si>
+    <t>2010 USD</t>
+  </si>
+  <si>
+    <t>OECD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;-- Source 3 (2014)</t>
+  </si>
+  <si>
+    <t>Source 2: http://www.isec.ac.in/WP%20407%20-%20Agamoni%20Majumder%20and%20Madheswaran%20-%20Final.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source 3: </t>
+  </si>
+  <si>
+    <t>Majumder&amp;Madheswaran use a new method, the hedonic wage approach, due to changes in the</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further, the OECD estimate (Source 3) uses a willingness-to-pay approach </t>
+  </si>
+  <si>
+    <t>(individuals' valuation of their willingness to pay to reduce the risk of dying)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to estimate the VSL for India, reported for the 2010 USD. This estimate is in a similar range as </t>
+  </si>
+  <si>
+    <t>Majumder &amp; Madheswaran's updated estimate (Source 2)</t>
+  </si>
+  <si>
+    <t>This is in the similar range as the OECD estimate (Source 3)</t>
+  </si>
+  <si>
+    <t>Source: 1)</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>3)</t>
+  </si>
+  <si>
+    <t>The Cost of Air Pollution: Health Impacts of Road Transport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +284,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +319,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -233,9 +350,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -250,7 +367,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -258,13 +375,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -282,6 +406,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>51586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>391577</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>106091</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D3D954E-A784-48D2-8CC8-CAA584E9A5DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="1956586"/>
+          <a:ext cx="5125502" cy="2721505"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29330</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{669BB9F7-1552-4FBD-B946-D12F07100D57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5267325" y="5591175"/>
+          <a:ext cx="5410955" cy="2867425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,6 +577,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -395,6 +629,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -570,105 +821,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="79.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2016</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>3</v>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{D3C99150-55C7-4300-A8DF-8B57DA819046}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -679,225 +1020,387 @@
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="16">
         <v>1999</v>
       </c>
-      <c r="C5">
+      <c r="C3" s="16">
         <f>AVERAGE(153000,358000)</f>
         <v>255500</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="17">
+        <f>C3*C15</f>
+        <v>352108.44537815126</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="16">
+        <v>2004</v>
+      </c>
+      <c r="C4" s="16">
+        <v>15000000</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="17">
+        <f>C4/B22*C16</f>
+        <v>418343.09938143368</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="16">
+        <v>2011</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3400000</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="17">
+        <f>C5*C14</f>
+        <v>5972605.9678653404</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="18">
+        <v>2018</v>
+      </c>
+      <c r="C6" s="18">
+        <f>44.69*10^6</f>
+        <v>44690000</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="19">
+        <f>C6/B23*C18</f>
+        <v>629154.80761072843</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="18">
+        <v>1997</v>
+      </c>
+      <c r="C7" s="18">
+        <f>AVERAGE(14,19)*10^6</f>
+        <v>16500000</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="18">
+        <v>2001</v>
+      </c>
+      <c r="C8" s="18">
+        <f>56*10^6</f>
+        <v>56000000</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2010</v>
+      </c>
+      <c r="C9" s="18">
+        <f>20*10^6</f>
+        <v>20000000</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="20">
+        <v>2014</v>
+      </c>
+      <c r="C10" s="20">
+        <f>0.602*10^6</f>
+        <v>602000</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="21">
+        <f>C10*C19</f>
+        <v>633853.63392889895</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="15">
-        <f>C5*C12</f>
-        <v>352660.54621848743</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B6">
+      <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1990</v>
+      </c>
+      <c r="B14" s="2">
+        <v>130.69999999999999</v>
+      </c>
+      <c r="C14" s="8">
+        <v>1.7566488140780414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1999</v>
+      </c>
+      <c r="B15" s="2">
+        <v>166.6</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1.3781152460984394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>2004</v>
       </c>
-      <c r="C6">
-        <v>15000000</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B16" s="2">
+        <v>188.9</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1.2154261514028586</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B17" s="2">
+        <v>229.59399999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B18" s="2">
+        <v>240.00700000000001</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.95661376543184151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B19" s="2">
+        <v>218.05600000000001</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1.0529130131709286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43.58</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="15">
-        <f>C6/B18*C13</f>
-        <v>418999.05518070247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>2011</v>
-      </c>
-      <c r="C7">
-        <v>3400000</v>
-      </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B23" s="2">
+        <v>67.95</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <f>E6</f>
+        <v>629154.80761072843</v>
+      </c>
+      <c r="B32" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="15">
-        <f>C7*C11</f>
-        <v>5981970.9257842395</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="12" t="s">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1990</v>
-      </c>
-      <c r="B11" s="2">
-        <v>130.69999999999999</v>
-      </c>
-      <c r="C11" s="8">
-        <v>1.7594032134659527</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1999</v>
-      </c>
-      <c r="B12" s="2">
-        <v>166.6</v>
-      </c>
-      <c r="C12" s="8">
-        <v>1.3802761104441779</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2004</v>
-      </c>
-      <c r="B13" s="2">
-        <v>188.9</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1.2173319216516676</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B14" s="2">
-        <v>229.95400000000001</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="2">
-        <v>43.58</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
-        <f>AVERAGE(E5:E6)</f>
-        <v>385829.80069959495</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>41</v>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="22" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A33" r:id="rId1"/>
+    <hyperlink ref="D47" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -907,16 +1410,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="14">
-        <f>'India Data'!A27</f>
-        <v>385829.80069959495</v>
+        <f>'India Data'!A32</f>
+        <v>629154.80761072843</v>
       </c>
     </row>
   </sheetData>

</xml_diff>